<commit_message>
sProd 되돌리고 key|Int 추가
</commit_message>
<xml_diff>
--- a/Excel/Shop.xlsx
+++ b/Excel/Shop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BCD1B-0E5D-4ED9-AFAD-B97F24A83E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155C55C8-7F3B-45CE-A975-FFF23897803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A95D980-8F25-43B6-BA87-364295A77694}"/>
+    <workbookView xWindow="-26850" yWindow="1935" windowWidth="13515" windowHeight="14265" xr2:uid="{1A95D980-8F25-43B6-BA87-364295A77694}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopProductTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
   <si>
     <t>productId|String</t>
   </si>
@@ -188,6 +188,63 @@
   </si>
   <si>
     <t>ev4_conti_8</t>
+  </si>
+  <si>
+    <t>key|Int</t>
+  </si>
+  <si>
+    <t>테이블연결</t>
+  </si>
+  <si>
+    <t>Jason화</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300}</t>
+  </si>
+  <si>
+    <t>{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300}</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300},{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80}</t>
+  </si>
+  <si>
+    <t>{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80}</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300},{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80},{"id":"ev4_conti_1","key":721,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":35000,"tp3":"cu","vl3":"EN","cn3":170}</t>
+  </si>
+  <si>
+    <t>{"id":"ev4_conti_1","key":721,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":35000,"tp3":"cu","vl3":"EN","cn3":170}</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300},{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80},{"id":"ev4_conti_1","key":721,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":35000,"tp3":"cu","vl3":"EN","cn3":170},{"id":"ev4_conti_2","key":884,"tp1":"cu","vl1":"EN","cn1":150}</t>
+  </si>
+  <si>
+    <t>{"id":"ev4_conti_2","key":884,"tp1":"cu","vl1":"EN","cn1":150}</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300},{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80},{"id":"ev4_conti_1","key":721,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":35000,"tp3":"cu","vl3":"EN","cn3":170},{"id":"ev4_conti_2","key":884,"tp1":"cu","vl1":"EN","cn1":150},{"id":"ev4_conti_4","key":394,"tp1":"cu","vl1":"EN","cn1":150,"tp2":"cu","vl2":"GO","cn2":20000}</t>
+  </si>
+  <si>
+    <t>{"id":"ev4_conti_4","key":394,"tp1":"cu","vl1":"EN","cn1":150,"tp2":"cu","vl2":"GO","cn2":20000}</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300},{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80},{"id":"ev4_conti_1","key":721,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":35000,"tp3":"cu","vl3":"EN","cn3":170},{"id":"ev4_conti_2","key":884,"tp1":"cu","vl1":"EN","cn1":150},{"id":"ev4_conti_4","key":394,"tp1":"cu","vl1":"EN","cn1":150,"tp2":"cu","vl2":"GO","cn2":20000},{"id":"ev4_conti_5","key":612,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":10000,"tp3":"cu","vl3":"EN","cn3":200}</t>
+  </si>
+  <si>
+    <t>{"id":"ev4_conti_5","key":612,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":10000,"tp3":"cu","vl3":"EN","cn3":200}</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300},{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80},{"id":"ev4_conti_1","key":721,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":35000,"tp3":"cu","vl3":"EN","cn3":170},{"id":"ev4_conti_2","key":884,"tp1":"cu","vl1":"EN","cn1":150},{"id":"ev4_conti_4","key":394,"tp1":"cu","vl1":"EN","cn1":150,"tp2":"cu","vl2":"GO","cn2":20000},{"id":"ev4_conti_5","key":612,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":10000,"tp3":"cu","vl3":"EN","cn3":200},{"id":"ev4_conti_7","key":930,"tp1":"cu","vl1":"GO","cn1":50000}</t>
+  </si>
+  <si>
+    <t>{"id":"ev4_conti_7","key":930,"tp1":"cu","vl1":"GO","cn1":50000}</t>
+  </si>
+  <si>
+    <t>,{"id":"ev5_oneplustwo_2","key":537,"tp1":"cu","vl1":"EN","cn1":300},{"id":"ev5_oneplustwo_3","key":314,"tp1":"cu","vl1":"EN","cn1":80},{"id":"ev4_conti_1","key":721,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":35000,"tp3":"cu","vl3":"EN","cn3":170},{"id":"ev4_conti_2","key":884,"tp1":"cu","vl1":"EN","cn1":150},{"id":"ev4_conti_4","key":394,"tp1":"cu","vl1":"EN","cn1":150,"tp2":"cu","vl2":"GO","cn2":20000},{"id":"ev4_conti_5","key":612,"tp1":"cu","vl1":"EN","cn1":80,"tp2":"cu","vl2":"GO","cn2":10000,"tp3":"cu","vl3":"EN","cn3":200},{"id":"ev4_conti_7","key":930,"tp1":"cu","vl1":"GO","cn1":50000},{"id":"ev4_conti_8","key":959,"tp1":"cu","vl1":"EN","cn1":350,"tp2":"cu","vl2":"GO","cn2":30000}</t>
+  </si>
+  <si>
+    <t>{"id":"ev4_conti_8","key":959,"tp1":"cu","vl1":"EN","cn1":350,"tp2":"cu","vl2":"GO","cn2":30000}</t>
   </si>
 </sst>
 </file>
@@ -551,11 +608,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED115DDC-E095-4A60-B3EA-80FAE0A4BDBC}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -563,14 +618,15 @@
     <col min="2" max="3" width="9.25" customWidth="1"/>
     <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" customWidth="1"/>
+    <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,52 +646,61 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -651,17 +716,20 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>434</v>
+      </c>
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -677,26 +745,29 @@
       <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
-        <v>24</v>
+      <c r="G3">
+        <v>806</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3">
         <v>600</v>
       </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
       <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -715,26 +786,29 @@
       <c r="F4" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>548</v>
+      </c>
+      <c r="H4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>30</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -744,17 +818,26 @@
       <c r="C5" t="b">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>24</v>
+      <c r="G5">
+        <v>537</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5">
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W5" t="s">
+        <v>53</v>
+      </c>
+      <c r="X5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -764,17 +847,26 @@
       <c r="C6" t="b">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
-        <v>24</v>
+      <c r="G6">
+        <v>314</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W6" t="s">
+        <v>55</v>
+      </c>
+      <c r="X6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -790,35 +882,41 @@
       <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="G7" t="s">
-        <v>24</v>
+      <c r="G7">
+        <v>876</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7">
         <v>30</v>
       </c>
-      <c r="J7" t="s">
-        <v>24</v>
-      </c>
       <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
         <v>26</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>25000</v>
       </c>
-      <c r="M7" t="s">
-        <v>24</v>
-      </c>
       <c r="N7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7">
+        <v>24</v>
+      </c>
+      <c r="O7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -834,35 +932,41 @@
       <c r="F8" t="s">
         <v>40</v>
       </c>
-      <c r="G8" t="s">
-        <v>24</v>
+      <c r="G8">
+        <v>973</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8">
         <v>60</v>
       </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
       <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
         <v>26</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>15000</v>
       </c>
-      <c r="M8" t="s">
-        <v>24</v>
-      </c>
       <c r="N8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -878,44 +982,50 @@
       <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
-        <v>24</v>
+      <c r="G9">
+        <v>180</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9">
         <v>90</v>
       </c>
-      <c r="J9" t="s">
-        <v>24</v>
-      </c>
       <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
         <v>26</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>30000</v>
       </c>
-      <c r="M9" t="s">
-        <v>24</v>
-      </c>
       <c r="N9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O9">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9">
         <v>150</v>
       </c>
-      <c r="P9" t="s">
-        <v>24</v>
-      </c>
       <c r="Q9" t="s">
-        <v>25</v>
-      </c>
-      <c r="R9">
+        <v>24</v>
+      </c>
+      <c r="R9" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9">
         <v>300</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -925,35 +1035,44 @@
       <c r="C10" t="b">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
-        <v>24</v>
+      <c r="G10">
+        <v>721</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10">
         <v>80</v>
       </c>
-      <c r="J10" t="s">
-        <v>24</v>
-      </c>
       <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
         <v>26</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>35000</v>
       </c>
-      <c r="M10" t="s">
-        <v>24</v>
-      </c>
       <c r="N10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O10">
+        <v>24</v>
+      </c>
+      <c r="O10" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W10" t="s">
+        <v>57</v>
+      </c>
+      <c r="X10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -963,17 +1082,26 @@
       <c r="C11" t="b">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>24</v>
+      <c r="G11">
+        <v>884</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W11" t="s">
+        <v>59</v>
+      </c>
+      <c r="X11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -992,44 +1120,50 @@
       <c r="F12" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="s">
-        <v>24</v>
+      <c r="G12">
+        <v>217</v>
       </c>
       <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>20000</v>
       </c>
-      <c r="J12" t="s">
-        <v>24</v>
-      </c>
       <c r="K12" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12">
         <v>150</v>
       </c>
-      <c r="M12" t="s">
-        <v>24</v>
-      </c>
       <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" t="s">
         <v>26</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>35000</v>
       </c>
-      <c r="P12" t="s">
-        <v>24</v>
-      </c>
       <c r="Q12" t="s">
-        <v>25</v>
-      </c>
-      <c r="R12">
+        <v>24</v>
+      </c>
+      <c r="R12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1039,26 +1173,35 @@
       <c r="C13" t="b">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
-        <v>24</v>
+      <c r="G13">
+        <v>394</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13">
         <v>150</v>
       </c>
-      <c r="J13" t="s">
-        <v>24</v>
-      </c>
       <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
         <v>26</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>20000</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W13" t="s">
+        <v>61</v>
+      </c>
+      <c r="X13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1068,35 +1211,44 @@
       <c r="C14" t="b">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
-        <v>24</v>
+      <c r="G14">
+        <v>612</v>
       </c>
       <c r="H14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14">
         <v>80</v>
       </c>
-      <c r="J14" t="s">
-        <v>24</v>
-      </c>
       <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" t="s">
         <v>26</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>10000</v>
       </c>
-      <c r="M14" t="s">
-        <v>24</v>
-      </c>
       <c r="N14" t="s">
-        <v>25</v>
-      </c>
-      <c r="O14">
+        <v>24</v>
+      </c>
+      <c r="O14" t="s">
+        <v>25</v>
+      </c>
+      <c r="P14">
         <v>200</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W14" t="s">
+        <v>63</v>
+      </c>
+      <c r="X14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1115,44 +1267,50 @@
       <c r="F15" t="s">
         <v>47</v>
       </c>
-      <c r="G15" t="s">
-        <v>24</v>
+      <c r="G15">
+        <v>501</v>
       </c>
       <c r="H15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15">
         <v>300</v>
       </c>
-      <c r="J15" t="s">
-        <v>24</v>
-      </c>
       <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" t="s">
         <v>26</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>25000</v>
       </c>
-      <c r="M15" t="s">
-        <v>24</v>
-      </c>
       <c r="N15" t="s">
-        <v>25</v>
-      </c>
-      <c r="O15">
+        <v>24</v>
+      </c>
+      <c r="O15" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15">
         <v>450</v>
       </c>
-      <c r="P15" t="s">
-        <v>24</v>
-      </c>
       <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" t="s">
         <v>26</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>35000</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1162,17 +1320,26 @@
       <c r="C16" t="b">
         <v>1</v>
       </c>
-      <c r="G16" t="s">
-        <v>24</v>
+      <c r="G16">
+        <v>930</v>
       </c>
       <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
         <v>26</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>50000</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="W16" t="s">
+        <v>65</v>
+      </c>
+      <c r="X16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1182,23 +1349,32 @@
       <c r="C17" t="b">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
-        <v>24</v>
+      <c r="G17">
+        <v>959</v>
       </c>
       <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17">
         <v>350</v>
       </c>
-      <c r="J17" t="s">
-        <v>24</v>
-      </c>
       <c r="K17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" t="s">
         <v>26</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>30000</v>
+      </c>
+      <c r="W17" t="s">
+        <v>67</v>
+      </c>
+      <c r="X17" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
컨슘 아이템에 Cash_sFortuneWheel 추가
</commit_message>
<xml_diff>
--- a/Excel/Shop.xlsx
+++ b/Excel/Shop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0670FD2-910A-42E2-AFC5-8350634FC120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B362E39-E30B-4A2C-AA36-D943ED675569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1A95D980-8F25-43B6-BA87-364295A77694}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="12345" windowHeight="8055" activeTab="2" xr2:uid="{1A95D980-8F25-43B6-BA87-364295A77694}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopProductTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="93">
   <si>
     <t>productId|String</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>CashName_sPetSale</t>
+  </si>
+  <si>
+    <t>Cash_sFortuneWheel</t>
+  </si>
+  <si>
+    <t>CashName_sFortuneWheel</t>
   </si>
 </sst>
 </file>
@@ -2794,10 +2800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A538EB96-EB04-4826-9AF0-A58A4FE56B38}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2830,6 +2836,14 @@
         <v>90</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
지정 아이템 Product_ 제거 및 Cash_sEquipTypeGacha411 샘플 적용해서 올림
</commit_message>
<xml_diff>
--- a/Excel/Shop.xlsx
+++ b/Excel/Shop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F85CC26-AE5B-4F94-8258-413373518DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880AE58A-10C1-4AC6-8F55-CC4E8A20799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1A95D980-8F25-43B6-BA87-364295A77694}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="239">
   <si>
     <t>productId|String</t>
   </si>
@@ -750,9 +750,6 @@
     <t>FreeStageAtk_04</t>
   </si>
   <si>
-    <t>Product_Equip030001</t>
-  </si>
-  <si>
     <t>Cash_sSpellGacha</t>
   </si>
   <si>
@@ -763,6 +760,12 @@
   </si>
   <si>
     <t>CashName_sSpell4Gacha</t>
+  </si>
+  <si>
+    <t>Equip030001</t>
+  </si>
+  <si>
+    <t>Cash_sEquipTypeGacha411</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1143,7 @@
   <dimension ref="A1:W125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A97" sqref="A97"/>
@@ -4819,31 +4822,31 @@
         <v>1</v>
       </c>
       <c r="L97" t="s">
+        <v>22</v>
+      </c>
+      <c r="M97" t="s">
+        <v>24</v>
+      </c>
+      <c r="N97">
+        <v>10000</v>
+      </c>
+      <c r="O97" t="s">
+        <v>22</v>
+      </c>
+      <c r="P97" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q97">
+        <v>120</v>
+      </c>
+      <c r="R97" t="s">
         <v>25</v>
       </c>
-      <c r="M97" t="s">
-        <v>233</v>
-      </c>
-      <c r="N97">
+      <c r="S97" t="s">
+        <v>237</v>
+      </c>
+      <c r="T97">
         <v>1</v>
-      </c>
-      <c r="O97" t="s">
-        <v>25</v>
-      </c>
-      <c r="P97" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q97">
-        <v>1</v>
-      </c>
-      <c r="R97" t="s">
-        <v>22</v>
-      </c>
-      <c r="S97" t="s">
-        <v>98</v>
-      </c>
-      <c r="T97">
-        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.3">
@@ -4896,13 +4899,13 @@
         <v>120</v>
       </c>
       <c r="R98" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="S98" t="s">
-        <v>98</v>
+        <v>238</v>
       </c>
       <c r="T98">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.3">
@@ -20413,18 +20416,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" t="s">
         <v>234</v>
-      </c>
-      <c r="B10" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" t="s">
         <v>236</v>
-      </c>
-      <c r="B11" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>